<commit_message>
feat: major pre-release update, see app first sheet
</commit_message>
<xml_diff>
--- a/db/NeoMedCont.xlsx
+++ b/db/NeoMedCont.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="145">
   <si>
     <t>mg</t>
   </si>
@@ -36,15 +36,6 @@
     <t>PROSTIN VR INF 0,5MG/ML AMP</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid alprostadil 0,5 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)
-• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml.
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd.
-• Etiketteer de injectiespuit(en).</t>
-  </si>
-  <si>
     <t>10-200 nanogram/kg/min</t>
   </si>
   <si>
@@ -54,16 +45,6 @@
     <t>CORDARONE  50MG/ML AMPUL 3 ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid amiodaron 50 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de amiodaron oplossing 50 mg/ml toe aan de glucose …...%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>5-15 microg/kg/min</t>
   </si>
   <si>
@@ -82,15 +63,6 @@
     <t xml:space="preserve">BUPIVACAINE 2.5 MG/ML FLACON 20ML </t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek de benodigde hoeveelheid bupivacaine 2,5 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid NaCl 0,9% op in een injectiespuit van 50 ml
-• Voeg de bupivacaine oplossing 2,5 mg/ml toe aan de NaCl 0,9%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>1 ml/kg/dag EPIDURAAL</t>
   </si>
   <si>
@@ -103,15 +75,6 @@
     <t>CATAPRESAN 0.15MG/ML AMPUL 1ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid clonidine 0,15 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is).
-• Vul aan met NaCl 0,9% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml.
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,25-2 microg/kg/uur</t>
   </si>
   <si>
@@ -121,16 +84,6 @@
     <t>DOBUTAMINE 12.5 MG/ML AMPUL 20ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid dobutamine 12,5 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de dobutamine oplossing 12,5 mg/ml toe aan de glucose ……%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>2-20 microg/kg/min</t>
   </si>
   <si>
@@ -140,15 +93,6 @@
     <t>DYNATRA DOPAMINE 40 MG/ML AMPUL 5ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid dopamine 40 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)
-• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>1-20 microg/kg/min</t>
   </si>
   <si>
@@ -161,13 +105,6 @@
     <t>DOPRAM 2 MG/ML INFUSIEZAK 500ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek de benodigde hoeveelheid doxapram 2 mg/ml op in een injectiespuit van 50 ml
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,5-2 mg/kg/uur</t>
   </si>
   <si>
@@ -177,10 +114,6 @@
     <t>FLOLAN 500 MICROG INFPDR + SOLV 2 X 50ML</t>
   </si>
   <si>
-    <t>Zie Iprova document:
-PP5231204_Epoprostenol Flolan iv</t>
-  </si>
-  <si>
     <t xml:space="preserve">5-40 nanogram/kg/min </t>
   </si>
   <si>
@@ -193,15 +126,6 @@
     <t>ESMOLOL HCL 10 MG/ML FLACON 10 ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek de benodigde hoeveelheid esmolol 10 mg/ml op in een injectiespuit van 50 ml.
-• Vul eventueel aan met glucose……% tot de aangevraagde hoeveelheid en meng.
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)
-V3.20171506.LF</t>
-  </si>
-  <si>
     <t>0,1-1 mg/kg/min</t>
   </si>
   <si>
@@ -214,17 +138,6 @@
     <t xml:space="preserve">FUROSEMIDE 10 MG/ML AMPUL 2 ML </t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid furosemide 10 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een gekleurde injectiespuit van 50 ml
-• Voeg de furosemide oplossing 10 mg/ml toe aan de glucose …...%
-• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)
-V3.20171506.LF</t>
-  </si>
-  <si>
     <t>1-4 mg/kg/dag</t>
   </si>
   <si>
@@ -240,12 +153,6 @@
     <t>INS NOVORAPID 100 IE/ML FLACON 10 ML</t>
   </si>
   <si>
-    <t>Zie Iprova documenten: 
-PP5231191_Insuline novorapid 0-6 IE in 12 ml Glucose 5% 
-PP5231192_Insuline novorapid 0-6 IE in 12 ml Glucose 10% 
-PP5231174_Insuline novorapid 0-6 IE in 12 ml NaCl 0,9%</t>
-  </si>
-  <si>
     <t>0,01-0,1 E/kg/uur</t>
   </si>
   <si>
@@ -255,15 +162,6 @@
     <t>ISOPRENALINE SULFAAT 1 MG = 1 ML INFC</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid isoprenaline 1,0 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)
-• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een gekleurde injectiespuit van 50 ml
-• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,01-1,5 microg/kg/min</t>
   </si>
   <si>
@@ -273,15 +171,6 @@
     <t>TRANDATE 5 MG/ML INJVLST 20 ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid labetalol 5 mg/ml op in een passende injectiespuit.
-• Vul eventueel aan met glucose……% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml.
-• Zuig lucht in de injectiespuit van 50 ml en meng.
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en).</t>
-  </si>
-  <si>
     <t>0,25-3 mg/kg/uur</t>
   </si>
   <si>
@@ -291,16 +180,6 @@
     <t>LIDOCAINE 2% AMPUL 5ML  (ZONDER CONSERV)</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid lidocaïne 20 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de lidocaïne oplossing 20 mg/ml toe aan de glucose …...%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t xml:space="preserve">5-7 mg/kg/uur </t>
   </si>
   <si>
@@ -310,16 +189,6 @@
     <t>MIDAZOLAM 5 MG/ML AMPUL 1 ML 3ML 10 ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid midazolam 5 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de midazolam oplossing 5 mg/ml toe aan de glucose …...%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,05-0,5 mg/kg/uur</t>
   </si>
   <si>
@@ -329,35 +198,12 @@
     <t>MILRINON 1 MG/ML AMPUL 10ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek de benodigde hoeveelheid milrinon 1 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de milrinon oplossing 1 mg/ml toe aan de glucose …...%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,25-0,75 microg/kg/min</t>
   </si>
   <si>
     <t>morfine</t>
   </si>
   <si>
-    <t>MORFINEHYDROCHLORIDE 5 MG = 5 ML EPIDURAAL/INTRATHECAAL</t>
-  </si>
-  <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid morfinehydrochloride 1 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de morfinehydrochloride oplossing 1 mg/ml toe aan de glucose …...%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,125-0,5 mg/kg/dag</t>
   </si>
   <si>
@@ -367,34 +213,12 @@
     <t>CARDENE 1MG/ML AMPUL 5ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid nicardipine 1 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een gekleurde injectiespuit van 50 ml
-• Voeg de nicardipine oplossing 1 mg/ml toe aan de glucose ……%
-• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,5 -2 microg/kg/min</t>
   </si>
   <si>
     <t>nitroprusside</t>
   </si>
   <si>
-    <t>NITROPRUSSIDE NATRIUM 50MG=5ML INJVLST</t>
-  </si>
-  <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid nitroprusside 10 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is).
-• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een gekleurde injectiespuit van 50 ml
-• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,5-8 microg/kg/min</t>
   </si>
   <si>
@@ -404,15 +228,6 @@
     <t>NORADRENALINE 1 MG/ML AMPUL 1ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek via een filternaald de benodigde hoeveelheid noradrenaline 1 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)
-• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een gekleurde injectiespuit van 50 ml.
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,05-2 microg/kg/min</t>
   </si>
   <si>
@@ -422,16 +237,6 @@
     <t>ROCURONIUM 10 MG/ML INJVLST FLACON 5 ML</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek de benodigde hoeveelheid rocuronium 10 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml
-• Voeg de rocuronium oplossing 10 mg/ml toe aan de glucose ……%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>0,3-2,2 mg/kg/uur</t>
   </si>
   <si>
@@ -441,16 +246,6 @@
     <t xml:space="preserve">SUFENTANIL 1 MICROG/ML + BUPIVAC 0.25% </t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D 
-• Trek de benodigde hoeveelheid sufentanil 1 µg/ml + bupivacaine 2,5 mg/ml op in een passende injectiespuit.
-• Trek de benodigde hoeveelheid NaCl 0,9% op in een injectiespuit van 50 ml
-• Voeg de sufentanil 1 µg/ml + bupivacaine 2,5 mg/ml oplossing toe aan de NaCl 0,9%
-• Zuig lucht in de injectiespuit van 50 ml en meng
-• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof.
-• Herhaal indien meerdere spuiten zijn aangevraagd
-• Etiketteer de injectiespuit(en)</t>
-  </si>
-  <si>
     <t>Medicamenten</t>
   </si>
   <si>
@@ -517,19 +312,11 @@
     <t>0,05-0,1 microg/kg/min</t>
   </si>
   <si>
-    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D
-·    Trek via een spike of filternaald 1 ml van het aangevraagde geneesmiddel op in een 1 ml injectiespuit (opgetrokken: …… ml).
-·    Trek 9 ml van het aangevraagde oplosmiddel op in een spuit van 10 ml (opgetrokken: …… ml)
-·    Voeg het geneesmiddel toe aan het oplosmiddel
-·    Zuig lucht in de injectiespuit van 10 ml en meng
-·    Ontlucht de spuit en sluit af met een rode afsluitdop
-·    Identificeer de spuit met het geneesmiddel en de verkregen concentratie. Gebruik deze spuit voor het vervolg.</t>
-  </si>
-  <si>
     <t>0,05 - 0,1 microg/kg/min</t>
   </si>
   <si>
     <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
 • Trek via een filternaald de benodigde hoeveelheid adrenaline 0,1 mg/ml op in een passende injectiespuit._x000D_
 • Trek de benodigde hoeveelheid glucose ……% op in een gekleurde injectiespuit van 50 ml._x000D_
 • Voeg de adrenaline oplossing 0,1 mg/ml toe aan de glucose …...%._x000D_
@@ -537,6 +324,297 @@
 • Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
 • Herhaal indien meerdere spuiten zijn aangevraagd._x000D_
 • Etiketteer de injectiespuit(en).</t>
+  </si>
+  <si>
+    <t>10 - 200 nanog/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek via een filternaald de benodigde hoeveelheid alprostadil 0,5 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)_x000D_
+• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml._x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd._x000D_
+• Etiketteer de injectiespuit(en).</t>
+  </si>
+  <si>
+    <t>5 - 15 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid amiodaron 50 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de amiodaron oplossing 50 mg/ml toe aan de glucose …...%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek de benodigde hoeveelheid bupivacaine 2,5 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid NaCl 0,9% op in een injectiespuit van 50 ml_x000D_
+• Voeg de bupivacaine oplossing 2,5 mg/ml toe aan de NaCl 0,9%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,25 - 2 microg/kg/uur</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid clonidine 0,15 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)._x000D_
+• Vul aan met NaCl 0,9% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml._x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>2 - 20 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek via een filternaald de benodigde hoeveelheid dobutamine 12,5 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de dobutamine oplossing 12,5 mg/ml toe aan de glucose ……%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>1 - 20 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid dopamine 40 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)_x000D_
+• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,5 - 2 mg/kg/uur</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek de benodigde hoeveelheid doxapram 2 mg/ml op in een injectiespuit van 50 ml_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>5 - 40 nanog/kg/min</t>
+  </si>
+  <si>
+    <t>Zie Iprova document:_x000D_
+PP5231204_Epoprostenol Flolan iv</t>
+  </si>
+  <si>
+    <t>0,1 - 1 mg/kg/min</t>
+  </si>
+  <si>
+    <t>1 - 4 mg/kg/dag</t>
+  </si>
+  <si>
+    <t>0,01 - 0,1 IE/kg/uur</t>
+  </si>
+  <si>
+    <t>0,01 - 1,5 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek via een filternaald de benodigde hoeveelheid isoprenaline 1,0 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)_x000D_
+• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een gekleurde injectiespuit van 50 ml_x000D_
+• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,25 - 3 mg/kg/uur</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid labetalol 5 mg/ml op in een passende injectiespuit._x000D_
+• Vul eventueel aan met glucose……% tot de aangevraagde hoeveelheid in een injectiespuit van 50 ml._x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng._x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en).</t>
+  </si>
+  <si>
+    <t>5 - 7 mg/kg/uur</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid lidocaïne 20 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de lidocaïne oplossing 20 mg/ml toe aan de glucose …...%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,05 - 5 mg/kg/uur</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid midazolam 5 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de midazolam oplossing 5 mg/ml toe aan de glucose …...%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,25 - 0,75 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek de benodigde hoeveelheid milrinon 1 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de milrinon oplossing 1 mg/ml toe aan de glucose …...%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,125 - 0,5 mg/kg/dag</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek via een filternaald de benodigde hoeveelheid morfinehydrochloride 1 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de morfinehydrochloride oplossing 1 mg/ml toe aan de glucose …...%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,5 - 2 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid nicardipine 1 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een gekleurde injectiespuit van 50 ml_x000D_
+• Voeg de nicardipine oplossing 1 mg/ml toe aan de glucose ……%_x000D_
+• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,5 - 8 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid nitroprusside 10 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)._x000D_
+• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een gekleurde injectiespuit van 50 ml_x000D_
+• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,05 - 2 microg/kg/min</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek via een filternaald de benodigde hoeveelheid noradrenaline 1 mg/ml of een 10-voudige hoeveelheid van de 1 op 10 verdunning* (=……..ml) op in een passende injectiespuit. (*doorhalen wat niet van toepassing is)_x000D_
+• Vul aan met glucose ……% tot de aangevraagde hoeveelheid in een gekleurde injectiespuit van 50 ml._x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>0,3 - 2,2 mg/kg/uur</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek de benodigde hoeveelheid rocuronium 10 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een injectiespuit van 50 ml_x000D_
+• Voeg de rocuronium oplossing 10 mg/ml toe aan de glucose ……%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE _x000D_
+• Trek de benodigde hoeveelheid sufentanil 1 µg/ml + bupivacaine 2,5 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid NaCl 0,9% op in een injectiespuit van 50 ml_x000D_
+• Voeg de sufentanil 1 µg/ml + bupivacaine 2,5 mg/ml oplossing toe aan de NaCl 0,9%_x000D_
+• Zuig lucht in de injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D_x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+·    Trek via een spike of filternaald 1 ml van het aangevraagde geneesmiddel op in een 1 ml injectiespuit (opgetrokken: …… ml)._x000D_
+·    Trek 9 ml van het aangevraagde oplosmiddel op in een spuit van 10 ml (opgetrokken: …… ml)_x000D_
+·    Voeg het geneesmiddel toe aan het oplosmiddel_x000D_
+·    Zuig lucht in de injectiespuit van 10 ml en meng_x000D_
+·    Ontlucht de spuit en sluit af met een rode afsluitdop_x000D_
+·    Identificeer de spuit met het geneesmiddel en de verkregen concentratie. Gebruik deze spuit voor het vervolg.</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek de benodigde hoeveelheid esmolol 10 mg/ml op in een injectiespuit van 50 ml._x000D_
+• Vul eventueel aan met glucose……% tot de aangevraagde hoeveelheid en meng._x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>WERK ASEPTISCH IN EEN VAN DE LAF-KASTEN met achtergrond klasse D _x000D_
+LINE CLEARANCE UITGEVOERD? JA/NEE_x000D_
+• Trek via een filternaald de benodigde hoeveelheid furosemide 10 mg/ml op in een passende injectiespuit._x000D_
+• Trek de benodigde hoeveelheid glucose ……% op in een gekleurde injectiespuit van 50 ml_x000D_
+• Voeg de furosemide oplossing 10 mg/ml toe aan de glucose …...%_x000D_
+• Zuig lucht in de gekleurde injectiespuit van 50 ml en meng_x000D_
+• Ontlucht de spuit en sluit af met een Cair LGL lijn. Vul de lijn met enkele centimeters vloeistof._x000D_
+• Herhaal indien meerdere spuiten zijn aangevraagd_x000D_
+• Etiketteer de injectiespuit(en)</t>
+  </si>
+  <si>
+    <t>Zie Iprova documenten: _x000D_
+PP5231174_Insuline novorapid 0-6 IE in 12 ml NaCl 0,9%</t>
+  </si>
+  <si>
+    <t>MORFINEHYDROCHLORIDE 1 MG/ML AMPUL 5ML EPIDURAAL/INTRATHECAAL</t>
+  </si>
+  <si>
+    <t>NITROPRUSSIDE NATRIUM 10 MG/ML INJVLST AMPUL 5ML</t>
   </si>
 </sst>
 </file>
@@ -967,67 +1045,67 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1060,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="M2" s="4">
         <v>12</v>
@@ -1069,7 +1147,7 @@
         <v>0.5</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="P2" s="4">
         <v>1</v>
@@ -1078,13 +1156,13 @@
         <v>2</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1196,9 @@
       <c r="K3" s="4">
         <v>3</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="M3" s="4">
         <v>12</v>
       </c>
@@ -1135,15 +1215,15 @@
         <v>2</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -1175,7 +1255,9 @@
       <c r="K4" s="4">
         <v>3</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="M4" s="4">
         <v>12</v>
       </c>
@@ -1183,30 +1265,30 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" s="5" t="s">
+    </row>
+    <row r="5" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -1233,7 +1315,7 @@
         <v>12</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M5" s="4">
         <v>24</v>
@@ -1242,30 +1324,30 @@
         <v>1</v>
       </c>
       <c r="O5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="5" t="s">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D6" s="3">
         <v>0.15</v>
@@ -1291,7 +1373,9 @@
       <c r="K6" s="4">
         <v>12</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="M6" s="4">
         <v>12</v>
       </c>
@@ -1299,7 +1383,7 @@
         <v>0.5</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P6" s="4">
         <v>1</v>
@@ -1308,15 +1392,15 @@
         <v>2</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -1348,7 +1432,9 @@
       <c r="K7" s="9">
         <v>3</v>
       </c>
-      <c r="L7" s="9"/>
+      <c r="L7" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="M7" s="9">
         <v>12</v>
       </c>
@@ -1356,7 +1442,7 @@
         <v>0.5</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P7" s="9">
         <v>1</v>
@@ -1365,15 +1451,15 @@
         <v>2</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -1405,7 +1491,9 @@
       <c r="K8" s="4">
         <v>3</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="M8" s="3">
         <v>12</v>
       </c>
@@ -1413,7 +1501,7 @@
         <v>0.5</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P8" s="3">
         <v>1</v>
@@ -1422,21 +1510,21 @@
         <v>2</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="6" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3">
         <v>2</v>
@@ -1462,7 +1550,9 @@
       <c r="K9" s="4">
         <v>1</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="M9" s="3">
         <v>12</v>
       </c>
@@ -1470,7 +1560,7 @@
         <v>0.5</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="P9" s="3">
         <v>1</v>
@@ -1479,15 +1569,15 @@
         <v>2</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -1519,7 +1609,9 @@
       <c r="K10" s="4">
         <v>1</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="M10" s="3">
         <v>12</v>
       </c>
@@ -1527,7 +1619,7 @@
         <v>0.5</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="P10" s="4">
         <v>1</v>
@@ -1536,21 +1628,21 @@
         <v>2</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -1576,7 +1668,9 @@
       <c r="K11" s="4">
         <v>3</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="M11" s="3">
         <v>12</v>
       </c>
@@ -1584,7 +1678,7 @@
         <v>0.5</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P11" s="4">
         <v>1</v>
@@ -1593,21 +1687,21 @@
         <v>2</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:20" s="6" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -1633,7 +1727,9 @@
       <c r="K12" s="4">
         <v>3</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="L12" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="M12" s="3">
         <v>12</v>
       </c>
@@ -1641,7 +1737,7 @@
         <v>0.5</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="P12" s="4">
         <v>1</v>
@@ -1650,21 +1746,21 @@
         <v>2</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1690,7 +1786,9 @@
       <c r="K13" s="4">
         <v>12</v>
       </c>
-      <c r="L13" s="4"/>
+      <c r="L13" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="M13" s="3">
         <v>12</v>
       </c>
@@ -1698,7 +1796,7 @@
         <v>0.5</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="P13" s="4">
         <v>1</v>
@@ -1707,15 +1805,15 @@
         <v>2</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -1747,7 +1845,9 @@
       <c r="K14" s="4">
         <v>3</v>
       </c>
-      <c r="L14" s="4"/>
+      <c r="L14" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="M14" s="3">
         <v>12</v>
       </c>
@@ -1755,7 +1855,7 @@
         <v>0.5</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="P14" s="4">
         <v>1</v>
@@ -1764,21 +1864,21 @@
         <v>2</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3">
         <v>5</v>
@@ -1804,7 +1904,9 @@
       <c r="K15" s="4">
         <v>3</v>
       </c>
-      <c r="L15" s="4"/>
+      <c r="L15" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="M15" s="3">
         <v>12</v>
       </c>
@@ -1812,7 +1914,7 @@
         <v>0.5</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="P15" s="4">
         <v>1</v>
@@ -1821,21 +1923,21 @@
         <v>2</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3">
         <v>20</v>
@@ -1861,7 +1963,9 @@
       <c r="K16" s="4">
         <v>3</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="M16" s="3">
         <v>48</v>
       </c>
@@ -1869,7 +1973,7 @@
         <v>2</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="P16" s="3">
         <v>1</v>
@@ -1878,21 +1982,21 @@
         <v>2</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3">
         <v>5</v>
@@ -1918,7 +2022,9 @@
       <c r="K17" s="4">
         <v>3</v>
       </c>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="M17" s="3">
         <v>12</v>
       </c>
@@ -1926,7 +2032,7 @@
         <v>0.5</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="P17" s="4">
         <v>1</v>
@@ -1935,15 +2041,15 @@
         <v>2</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
@@ -1975,7 +2081,9 @@
       <c r="K18" s="4">
         <v>3</v>
       </c>
-      <c r="L18" s="4"/>
+      <c r="L18" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="M18" s="3">
         <v>12</v>
       </c>
@@ -1983,7 +2091,7 @@
         <v>0.5</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="P18" s="4">
         <v>1</v>
@@ -1992,21 +2100,21 @@
         <v>2</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -2032,7 +2140,9 @@
       <c r="K19" s="4">
         <v>3</v>
       </c>
-      <c r="L19" s="4"/>
+      <c r="L19" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="M19" s="3">
         <v>12</v>
       </c>
@@ -2040,7 +2150,7 @@
         <v>0.5</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="P19" s="4">
         <v>1</v>
@@ -2049,15 +2159,15 @@
         <v>2</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>0</v>
@@ -2089,7 +2199,9 @@
       <c r="K20" s="4">
         <v>3</v>
       </c>
-      <c r="L20" s="4"/>
+      <c r="L20" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="M20" s="3">
         <v>12</v>
       </c>
@@ -2097,7 +2209,7 @@
         <v>0.5</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="P20" s="4">
         <v>1</v>
@@ -2106,15 +2218,15 @@
         <v>2</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -2146,7 +2258,9 @@
       <c r="K21" s="4">
         <v>3</v>
       </c>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="M21" s="3">
         <v>12</v>
       </c>
@@ -2154,7 +2268,7 @@
         <v>0.5</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="P21" s="4">
         <v>1</v>
@@ -2163,15 +2277,15 @@
         <v>2</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
@@ -2203,7 +2317,9 @@
       <c r="K22" s="4">
         <v>3</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="M22" s="3">
         <v>12</v>
       </c>
@@ -2211,7 +2327,7 @@
         <v>0.5</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="P22" s="4">
         <v>1</v>
@@ -2220,21 +2336,21 @@
         <v>2</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D23" s="3">
         <v>10</v>
@@ -2260,7 +2376,9 @@
       <c r="K23" s="4">
         <v>3</v>
       </c>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="M23" s="3">
         <v>12</v>
       </c>
@@ -2268,7 +2386,7 @@
         <v>0.5</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="P23" s="4">
         <v>1</v>
@@ -2277,21 +2395,21 @@
         <v>2</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -2318,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M24" s="6">
         <v>24</v>
@@ -2327,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="P24" s="6">
         <v>1</v>
@@ -2336,10 +2454,10 @@
         <v>2</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2363,9 +2481,9 @@
     <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: number of bug fixes
</commit_message>
<xml_diff>
--- a/db/NeoMedCont.xlsx
+++ b/db/NeoMedCont.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Tbl_Admin_NeoMedCont" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>5-15 microg/kg/min</t>
   </si>
   <si>
-    <t>bupivacaine EPIDURAAL</t>
-  </si>
-  <si>
     <t>ml</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
   </si>
   <si>
     <t>0,3-2,2 mg/kg/uur</t>
-  </si>
-  <si>
-    <t>sufentanil/bupivac EPIDURAAL</t>
   </si>
   <si>
     <t xml:space="preserve">SUFENTANIL 1 MICROG/ML + BUPIVAC 0.25% </t>
@@ -615,6 +609,12 @@
   </si>
   <si>
     <t>NITROPRUSSIDE NATRIUM 10 MG/ML INJVLST AMPUL 5ML</t>
+  </si>
+  <si>
+    <t>bupivacaine 0,25% EPI</t>
+  </si>
+  <si>
+    <t>sufenta 1 mcg/ml bupivac 0,25% EPI</t>
   </si>
 </sst>
 </file>
@@ -1025,11 +1025,11 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,67 +1045,67 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1138,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M2" s="4">
         <v>12</v>
@@ -1147,7 +1147,7 @@
         <v>0.5</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P2" s="4">
         <v>1</v>
@@ -1156,10 +1156,10 @@
         <v>2</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M3" s="4">
         <v>12</v>
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>6</v>
@@ -1256,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M4" s="4">
         <v>12</v>
@@ -1274,7 +1274,7 @@
         <v>2</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>9</v>
@@ -1282,14 +1282,14 @@
     </row>
     <row r="5" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="4">
-        <v>1.01</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
@@ -1315,7 +1315,7 @@
         <v>12</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M5" s="4">
         <v>24</v>
@@ -1324,30 +1324,30 @@
         <v>1</v>
       </c>
       <c r="O5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="P5" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>0.15</v>
@@ -1374,7 +1374,7 @@
         <v>12</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M6" s="4">
         <v>12</v>
@@ -1383,24 +1383,24 @@
         <v>0.5</v>
       </c>
       <c r="O6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="P6" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -1433,7 +1433,7 @@
         <v>3</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M7" s="9">
         <v>12</v>
@@ -1442,24 +1442,24 @@
         <v>0.5</v>
       </c>
       <c r="O7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="P7" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M8" s="3">
         <v>12</v>
@@ -1501,30 +1501,30 @@
         <v>0.5</v>
       </c>
       <c r="O8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="S8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="P8" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D9" s="3">
         <v>2</v>
@@ -1551,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M9" s="3">
         <v>12</v>
@@ -1560,24 +1560,24 @@
         <v>0.5</v>
       </c>
       <c r="O9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="P9" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M10" s="3">
         <v>12</v>
@@ -1619,30 +1619,30 @@
         <v>0.5</v>
       </c>
       <c r="O10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="S10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="P10" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -1669,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M11" s="3">
         <v>12</v>
@@ -1678,30 +1678,30 @@
         <v>0.5</v>
       </c>
       <c r="O11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S11" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -1728,7 +1728,7 @@
         <v>3</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M12" s="3">
         <v>12</v>
@@ -1737,30 +1737,30 @@
         <v>0.5</v>
       </c>
       <c r="O12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="S12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="P12" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1787,7 +1787,7 @@
         <v>12</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M13" s="3">
         <v>12</v>
@@ -1796,24 +1796,24 @@
         <v>0.5</v>
       </c>
       <c r="O13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P13" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="P13" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -1846,7 +1846,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M14" s="3">
         <v>12</v>
@@ -1855,30 +1855,30 @@
         <v>0.5</v>
       </c>
       <c r="O14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P14" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="S14" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="P14" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3">
         <v>5</v>
@@ -1905,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M15" s="3">
         <v>12</v>
@@ -1914,30 +1914,30 @@
         <v>0.5</v>
       </c>
       <c r="O15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="S15" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="P15" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3">
         <v>20</v>
@@ -1964,7 +1964,7 @@
         <v>3</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M16" s="3">
         <v>48</v>
@@ -1973,30 +1973,30 @@
         <v>2</v>
       </c>
       <c r="O16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="S16" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="P16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3">
         <v>5</v>
@@ -2023,7 +2023,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M17" s="3">
         <v>12</v>
@@ -2032,24 +2032,24 @@
         <v>0.5</v>
       </c>
       <c r="O17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="P17" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
@@ -2082,7 +2082,7 @@
         <v>3</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M18" s="3">
         <v>12</v>
@@ -2091,30 +2091,30 @@
         <v>0.5</v>
       </c>
       <c r="O18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="P18" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M19" s="3">
         <v>12</v>
@@ -2150,7 +2150,7 @@
         <v>0.5</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P19" s="4">
         <v>1</v>
@@ -2159,15 +2159,15 @@
         <v>2</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>3</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M20" s="3">
         <v>12</v>
@@ -2209,24 +2209,24 @@
         <v>0.5</v>
       </c>
       <c r="O20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="S20" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="P20" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -2259,7 +2259,7 @@
         <v>3</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M21" s="3">
         <v>12</v>
@@ -2268,7 +2268,7 @@
         <v>0.5</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P21" s="4">
         <v>1</v>
@@ -2277,15 +2277,15 @@
         <v>2</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
@@ -2318,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M22" s="3">
         <v>12</v>
@@ -2327,30 +2327,30 @@
         <v>0.5</v>
       </c>
       <c r="O22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="P22" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="3">
         <v>10</v>
@@ -2377,7 +2377,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M23" s="3">
         <v>12</v>
@@ -2386,31 +2386,31 @@
         <v>0.5</v>
       </c>
       <c r="O23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="S23" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="P23" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="D24" s="6">
         <v>1</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="6">
-        <v>1.01</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="I24" s="6">
         <v>0</v>
@@ -2436,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M24" s="6">
         <v>24</v>
@@ -2445,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P24" s="6">
         <v>1</v>
@@ -2454,10 +2454,10 @@
         <v>2</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +2473,7 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2483,7 +2483,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: nieuwe epiduralen en discontinue medicatie formulier, voorbereiding op volgende release
</commit_message>
<xml_diff>
--- a/db/NeoMedCont.xlsx
+++ b/db/NeoMedCont.xlsx
@@ -60,9 +60,6 @@
     <t xml:space="preserve">BUPIVACAINE 2.5 MG/ML FLACON 20ML </t>
   </si>
   <si>
-    <t>1 ml/kg/dag EPIDURAAL</t>
-  </si>
-  <si>
     <t>clonidine</t>
   </si>
   <si>
@@ -611,10 +608,13 @@
     <t>NITROPRUSSIDE NATRIUM 10 MG/ML INJVLST AMPUL 5ML</t>
   </si>
   <si>
-    <t>bupivacaine 0,25% EPI</t>
-  </si>
-  <si>
-    <t>sufenta 1 mcg/ml bupivac 0,25% EPI</t>
+    <t>bupivacaine 0,125% EPI</t>
+  </si>
+  <si>
+    <t>2 ml/kg/dag EPIDURAAL</t>
+  </si>
+  <si>
+    <t>sufenta 0,5 mcg/ml bupivac 0,125% EPI</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1029,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,67 +1045,67 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1138,7 +1138,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M2" s="4">
         <v>12</v>
@@ -1147,19 +1147,19 @@
         <v>0.5</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="P2" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -1197,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M3" s="4">
         <v>12</v>
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>6</v>
@@ -1256,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M4" s="4">
         <v>12</v>
@@ -1274,7 +1274,7 @@
         <v>2</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>9</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="5" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
@@ -1297,13 +1297,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="4">
-        <v>2.0099999999999998</v>
+        <v>4.01</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
@@ -1333,21 +1333,21 @@
         <v>2</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="3">
         <v>0.15</v>
@@ -1374,7 +1374,7 @@
         <v>12</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M6" s="4">
         <v>12</v>
@@ -1383,24 +1383,24 @@
         <v>0.5</v>
       </c>
       <c r="O6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="P6" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -1433,7 +1433,7 @@
         <v>3</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M7" s="9">
         <v>12</v>
@@ -1442,24 +1442,24 @@
         <v>0.5</v>
       </c>
       <c r="O7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="P7" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M8" s="3">
         <v>12</v>
@@ -1501,30 +1501,30 @@
         <v>0.5</v>
       </c>
       <c r="O8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="S8" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="P8" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="6" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="3">
         <v>2</v>
@@ -1551,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M9" s="3">
         <v>12</v>
@@ -1560,24 +1560,24 @@
         <v>0.5</v>
       </c>
       <c r="O9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="P9" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M10" s="3">
         <v>12</v>
@@ -1619,30 +1619,30 @@
         <v>0.5</v>
       </c>
       <c r="O10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="S10" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="P10" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -1669,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M11" s="3">
         <v>12</v>
@@ -1678,30 +1678,30 @@
         <v>0.5</v>
       </c>
       <c r="O11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="S11" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="P11" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="D12" s="3">
         <v>10</v>
@@ -1728,7 +1728,7 @@
         <v>3</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M12" s="3">
         <v>12</v>
@@ -1737,30 +1737,30 @@
         <v>0.5</v>
       </c>
       <c r="O12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S12" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="P12" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -1787,7 +1787,7 @@
         <v>12</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M13" s="3">
         <v>12</v>
@@ -1796,24 +1796,24 @@
         <v>0.5</v>
       </c>
       <c r="O13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P13" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="P13" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -1846,7 +1846,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M14" s="3">
         <v>12</v>
@@ -1855,30 +1855,30 @@
         <v>0.5</v>
       </c>
       <c r="O14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="S14" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="P14" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R14" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="S14" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3">
         <v>5</v>
@@ -1905,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M15" s="3">
         <v>12</v>
@@ -1914,30 +1914,30 @@
         <v>0.5</v>
       </c>
       <c r="O15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="S15" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="P15" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="3">
         <v>20</v>
@@ -1964,7 +1964,7 @@
         <v>3</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M16" s="3">
         <v>48</v>
@@ -1973,30 +1973,30 @@
         <v>2</v>
       </c>
       <c r="O16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="S16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="P16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="3">
         <v>5</v>
@@ -2023,7 +2023,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M17" s="3">
         <v>12</v>
@@ -2032,24 +2032,24 @@
         <v>0.5</v>
       </c>
       <c r="O17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="P17" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
@@ -2082,7 +2082,7 @@
         <v>3</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M18" s="3">
         <v>12</v>
@@ -2091,30 +2091,30 @@
         <v>0.5</v>
       </c>
       <c r="O18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="P18" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M19" s="3">
         <v>12</v>
@@ -2150,7 +2150,7 @@
         <v>0.5</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P19" s="4">
         <v>1</v>
@@ -2159,15 +2159,15 @@
         <v>2</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>3</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M20" s="3">
         <v>12</v>
@@ -2209,24 +2209,24 @@
         <v>0.5</v>
       </c>
       <c r="O20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="S20" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="P20" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>0</v>
@@ -2259,7 +2259,7 @@
         <v>3</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M21" s="3">
         <v>12</v>
@@ -2268,7 +2268,7 @@
         <v>0.5</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P21" s="4">
         <v>1</v>
@@ -2277,15 +2277,15 @@
         <v>2</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>0</v>
@@ -2318,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M22" s="3">
         <v>12</v>
@@ -2327,30 +2327,30 @@
         <v>0.5</v>
       </c>
       <c r="O22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="P22" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="3">
         <v>10</v>
@@ -2377,7 +2377,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M23" s="3">
         <v>12</v>
@@ -2386,19 +2386,19 @@
         <v>0.5</v>
       </c>
       <c r="O23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P23" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="S23" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="P23" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R23" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -2418,13 +2418,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24" s="6">
-        <v>2.0099999999999998</v>
+        <v>4.01</v>
       </c>
       <c r="I24" s="6">
         <v>0</v>
@@ -2445,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P24" s="6">
         <v>1</v>
@@ -2454,10 +2454,10 @@
         <v>2</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2483,7 +2483,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: med disc database save and load
</commit_message>
<xml_diff>
--- a/db/NeoMedCont.xlsx
+++ b/db/NeoMedCont.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Tbl_Admin_NeoMedCont">Tbl_Admin_NeoMedCont!$A$2:$R$24</definedName>
+    <definedName name="Tbl_Admin_NeoMedCont">Tbl_Admin_NeoMedCont!$A$2:$S$24</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
   <si>
     <t>mg</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>NITROPRUSSIDE NATRIUM 25 MG/ML INJVLST AMPUL 2ML</t>
+  </si>
+  <si>
+    <t>OplVl Verplicht</t>
   </si>
 </sst>
 </file>
@@ -899,10 +902,10 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +974,9 @@
       <c r="R1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="1"/>
+      <c r="S1" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="2" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1026,6 +1031,9 @@
       <c r="R2" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="S2" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1080,6 +1088,9 @@
       <c r="R3" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="S3" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1134,6 +1145,9 @@
       <c r="R4" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="S4" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1190,6 +1204,9 @@
       <c r="R5" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="S5" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1244,6 +1261,9 @@
       <c r="R6" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="S6" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1298,6 +1318,9 @@
       <c r="R7" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="S7" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:19" s="6" customFormat="1" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1352,6 +1375,9 @@
       <c r="R8" s="12" t="s">
         <v>74</v>
       </c>
+      <c r="S8" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1406,6 +1432,9 @@
       <c r="R9" s="12" t="s">
         <v>99</v>
       </c>
+      <c r="S9" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1460,6 +1489,9 @@
       <c r="R10" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="S10" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:19" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1514,6 +1546,9 @@
       <c r="R11" s="5" t="s">
         <v>86</v>
       </c>
+      <c r="S11" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1568,6 +1603,9 @@
       <c r="R12" s="5" t="s">
         <v>87</v>
       </c>
+      <c r="S12" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1622,6 +1660,9 @@
       <c r="R13" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="S13" s="6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -1676,6 +1717,9 @@
       <c r="R14" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="S14" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:19" s="6" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1730,6 +1774,9 @@
       <c r="R15" s="5" t="s">
         <v>77</v>
       </c>
+      <c r="S15" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:19" s="6" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1784,8 +1831,11 @@
       <c r="R16" s="12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S16" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>37</v>
       </c>
@@ -1838,8 +1888,11 @@
       <c r="R17" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S17" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>39</v>
       </c>
@@ -1892,8 +1945,11 @@
       <c r="R18" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S18" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>41</v>
       </c>
@@ -1946,8 +2002,11 @@
       <c r="R19" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S19" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
@@ -2000,8 +2059,11 @@
       <c r="R20" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S20" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>44</v>
       </c>
@@ -2054,8 +2116,11 @@
       <c r="R21" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S21" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
@@ -2108,8 +2173,11 @@
       <c r="R22" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S22" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
@@ -2162,8 +2230,11 @@
       <c r="R23" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="S23" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="6" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>91</v>
       </c>
@@ -2217,6 +2288,9 @@
       </c>
       <c r="R24" s="14" t="s">
         <v>92</v>
+      </c>
+      <c r="S24" s="6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>